<commit_message>
I added the hang man pics and the layout and started with the main coding aspect
</commit_message>
<xml_diff>
--- a/list of animals for hang man.xlsx
+++ b/list of animals for hang man.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taran\Documents\courses\Semester 4\Mobile Project\VictorLooksAmazing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEBF8806-8B56-4D9B-ABAA-40AB4F4A0815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2589D7A-074A-484D-BFBF-17A0AEDD00C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C1BA2B30-831B-4B39-B50C-D432F0936D09}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Animals</t>
   </si>
@@ -42,62 +42,111 @@
     <t>Activities</t>
   </si>
   <si>
-    <t>Ant</t>
-  </si>
-  <si>
-    <t>Anteater</t>
-  </si>
-  <si>
-    <t>Antelope</t>
-  </si>
-  <si>
-    <t>Armadillo</t>
-  </si>
-  <si>
-    <t>Baboon</t>
-  </si>
-  <si>
-    <t>Badger</t>
-  </si>
-  <si>
-    <t>Barracuda</t>
-  </si>
-  <si>
-    <t>Bat</t>
-  </si>
-  <si>
-    <t>Bear</t>
-  </si>
-  <si>
-    <t>Beaver</t>
-  </si>
-  <si>
-    <t>Beetle</t>
-  </si>
-  <si>
-    <t>Bird</t>
-  </si>
-  <si>
-    <t>Blue Whale</t>
-  </si>
-  <si>
-    <t>Buffalo</t>
+    <t>MOKNEY</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>DOG</t>
+  </si>
+  <si>
+    <t>BIRD</t>
+  </si>
+  <si>
+    <t>HIPPO</t>
+  </si>
+  <si>
+    <t>COW</t>
+  </si>
+  <si>
+    <t>HORSE</t>
+  </si>
+  <si>
+    <t>WHALE</t>
+  </si>
+  <si>
+    <t>TURTLE</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>GOAT</t>
+  </si>
+  <si>
+    <t>RABBIT</t>
+  </si>
+  <si>
+    <t>SNAKE</t>
+  </si>
+  <si>
+    <t>SKI</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>JUMP</t>
+  </si>
+  <si>
+    <t>SING</t>
+  </si>
+  <si>
+    <t>DANCE</t>
+  </si>
+  <si>
+    <t>WRITE</t>
+  </si>
+  <si>
+    <t>DRIVE</t>
+  </si>
+  <si>
+    <t>BIKE</t>
+  </si>
+  <si>
+    <t>PARTY</t>
+  </si>
+  <si>
+    <t>EAT</t>
+  </si>
+  <si>
+    <t>DRINK</t>
+  </si>
+  <si>
+    <t>CLEAN</t>
+  </si>
+  <si>
+    <t>STUDY</t>
+  </si>
+  <si>
+    <t>DIE</t>
+  </si>
+  <si>
+    <t>QUARANTINE</t>
+  </si>
+  <si>
+    <t>COVID</t>
+  </si>
+  <si>
+    <t>CORONA</t>
+  </si>
+  <si>
+    <t>BLACK LIVES MATTER</t>
+  </si>
+  <si>
+    <t>WWIII</t>
+  </si>
+  <si>
+    <t>RHINO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,7 +176,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D04146-A6CF-4523-9840-97100D310B9E}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,70 +514,127 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>15</v>
+      <c r="B15" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>